<commit_message>
Added basic maps for Castle Never to start improving
</commit_message>
<xml_diff>
--- a/A1 - Downtime Activities/1b - Piety - Renown/Renown Tracker.xlsx
+++ b/A1 - Downtime Activities/1b - Piety - Renown/Renown Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachv\repos\NeverwinterNights\A1 - Downtime Activities\1b - Piety - Renown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E8359-2D90-4C82-87F4-D0E5676BF5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD89E78-0F53-46B8-8958-A1E015E1279C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="24180" windowHeight="15820" xr2:uid="{7374F566-E16E-4CAA-91ED-5366448EAD2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7374F566-E16E-4CAA-91ED-5366448EAD2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>Acholyte / Man at arms</t>
-  </si>
-  <si>
-    <t>Deacon / Squire</t>
-  </si>
-  <si>
     <t>Priest / Bachelor Knight</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>Stacia</t>
+  </si>
+  <si>
+    <t>Deacon / Knight</t>
+  </si>
+  <si>
+    <t>Acholyte / Squires</t>
   </si>
 </sst>
 </file>
@@ -173,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -319,7 +319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F386D783-C8F3-4907-BF9A-797E6FF055AA}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -518,10 +518,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -569,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -577,10 +577,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -596,7 +596,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -612,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -628,7 +628,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -636,7 +636,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -644,7 +644,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -660,10 +660,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -671,7 +671,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -687,7 +687,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -735,7 +735,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -743,10 +743,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -786,7 +786,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,7 +818,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -826,10 +826,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -837,7 +837,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -845,7 +845,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -861,7 +861,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -877,7 +877,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,7 +893,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -901,7 +901,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -909,10 +909,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +933,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>